<commit_message>
updated nav stress processing script but it's not done yet, far from it
also updated an OA list
</commit_message>
<xml_diff>
--- a/outputs/complete_lists/Older Adults/OA S017.xlsx
+++ b/outputs/complete_lists/Older Adults/OA S017.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amuller\Desktop\Alana\UA\R_projects\inflatable-project\outputs\complete_lists\Older Adults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{297B4BFB-2222-4B4A-86D3-9FA44809E4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FF830F-30A7-4F1E-9DFC-5E2518A3BC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10490" yWindow="1030" windowWidth="26200" windowHeight="18260"/>
+    <workbookView xWindow="3290" yWindow="240" windowWidth="28190" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ten_lists" sheetId="1" r:id="rId1"/>
@@ -430,13 +430,13 @@
     <t>no walk/diff</t>
   </si>
   <si>
-    <t>S000</t>
+    <t>S017 OA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1286,19 +1286,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32:K36"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="1.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2.81640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
@@ -1316,7 +1318,7 @@
         <v>132</v>
       </c>
       <c r="I3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -1457,7 +1459,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I10" t="s">
         <v>134</v>
@@ -1601,10 +1603,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -1745,7 +1747,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I24" t="s">
         <v>132</v>
@@ -1889,7 +1891,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C31" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I31" t="s">
         <v>135</v>

</xml_diff>